<commit_message>
amended small and medium test cases
</commit_message>
<xml_diff>
--- a/Python/tests/grids.xlsx
+++ b/Python/tests/grids.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\fe_assignment\Python\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF88500-F262-493C-8942-D9F7820D4301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166A7730-2576-4B3A-8512-EB3F98AE4D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="15600" activeTab="3" xr2:uid="{B1DB6A6A-67B5-44D5-9085-20B34B44A397}"/>
+    <workbookView xWindow="-28755" yWindow="285" windowWidth="20910" windowHeight="15195" activeTab="3" xr2:uid="{B1DB6A6A-67B5-44D5-9085-20B34B44A397}"/>
   </bookViews>
   <sheets>
     <sheet name="SmallGrid" sheetId="2" r:id="rId1"/>
@@ -104,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -113,9 +113,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -455,7 +452,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +485,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="2"/>
@@ -500,7 +497,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -520,7 +517,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +707,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +830,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="6"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -849,7 +846,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="1"/>
       <c r="I8" s="4"/>
@@ -865,7 +862,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="4"/>
@@ -928,7 +925,7 @@
   <dimension ref="A2:AG79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="AK26" sqref="AK26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
amended test cases to include deflections and changed logic to parse rays for two digit numbers and above.
</commit_message>
<xml_diff>
--- a/Python/tests/grids.xlsx
+++ b/Python/tests/grids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\fe_assignment\Python\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166A7730-2576-4B3A-8512-EB3F98AE4D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6123FA9E-72B7-4ED9-99F9-C695451E06D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28755" yWindow="285" windowWidth="20910" windowHeight="15195" activeTab="3" xr2:uid="{B1DB6A6A-67B5-44D5-9085-20B34B44A397}"/>
   </bookViews>
@@ -922,10 +922,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75C6D46-B383-4768-91A8-7C1DC67E6F96}">
-  <dimension ref="A2:AG79"/>
+  <dimension ref="A2:AG34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK26" sqref="AK26"/>
+      <selection activeCell="AK30" sqref="AK30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1094,7 @@
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AG4" s="2"/>
     </row>
@@ -1295,7 +1295,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1314,7 +1314,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
@@ -1532,7 +1532,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
@@ -1714,7 +1714,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P21" s="1"/>
       <c r="Q21" s="3"/>
@@ -1824,7 +1824,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1834,7 +1834,7 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
@@ -2046,7 +2046,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2221,1294 +2221,6 @@
       <c r="AF34" s="2"/>
       <c r="AG34" s="1"/>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>2</v>
-      </c>
-      <c r="E47">
-        <v>3</v>
-      </c>
-      <c r="F47">
-        <v>4</v>
-      </c>
-      <c r="G47">
-        <v>5</v>
-      </c>
-      <c r="H47">
-        <v>6</v>
-      </c>
-      <c r="I47">
-        <v>7</v>
-      </c>
-      <c r="J47">
-        <v>8</v>
-      </c>
-      <c r="K47">
-        <v>9</v>
-      </c>
-      <c r="L47">
-        <v>10</v>
-      </c>
-      <c r="M47">
-        <v>11</v>
-      </c>
-      <c r="N47">
-        <v>12</v>
-      </c>
-      <c r="O47">
-        <v>13</v>
-      </c>
-      <c r="P47">
-        <v>14</v>
-      </c>
-      <c r="Q47">
-        <v>15</v>
-      </c>
-      <c r="R47">
-        <v>16</v>
-      </c>
-      <c r="S47">
-        <v>17</v>
-      </c>
-      <c r="T47">
-        <v>18</v>
-      </c>
-      <c r="U47">
-        <v>19</v>
-      </c>
-      <c r="V47">
-        <v>20</v>
-      </c>
-      <c r="W47">
-        <v>21</v>
-      </c>
-      <c r="X47">
-        <v>22</v>
-      </c>
-      <c r="Y47">
-        <v>23</v>
-      </c>
-      <c r="Z47">
-        <v>24</v>
-      </c>
-      <c r="AA47">
-        <v>25</v>
-      </c>
-      <c r="AB47">
-        <v>26</v>
-      </c>
-      <c r="AC47">
-        <v>27</v>
-      </c>
-      <c r="AD47">
-        <v>28</v>
-      </c>
-      <c r="AE47">
-        <v>29</v>
-      </c>
-      <c r="AF47">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
-      <c r="X48" s="2"/>
-      <c r="Y48" s="2"/>
-      <c r="Z48" s="2"/>
-      <c r="AA48" s="2"/>
-      <c r="AB48" s="2"/>
-      <c r="AC48" s="2"/>
-      <c r="AD48" s="2"/>
-      <c r="AE48" s="2"/>
-      <c r="AF48" s="2"/>
-      <c r="AG48" s="1"/>
-    </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-      <c r="W49" s="1"/>
-      <c r="X49" s="1"/>
-      <c r="Y49" s="1"/>
-      <c r="Z49" s="1"/>
-      <c r="AA49" s="1"/>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="1"/>
-      <c r="AD49" s="1"/>
-      <c r="AE49" s="1"/>
-      <c r="AF49" s="5">
-        <v>3</v>
-      </c>
-      <c r="AG49" s="2"/>
-    </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>2</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
-      <c r="W50" s="1"/>
-      <c r="X50" s="1"/>
-      <c r="Y50" s="1"/>
-      <c r="Z50" s="1"/>
-      <c r="AA50" s="1"/>
-      <c r="AB50" s="1"/>
-      <c r="AC50" s="1"/>
-      <c r="AD50" s="1"/>
-      <c r="AE50" s="1"/>
-      <c r="AF50" s="1"/>
-      <c r="AG50" s="2"/>
-    </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>3</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
-      <c r="S51" s="1"/>
-      <c r="T51" s="1"/>
-      <c r="U51" s="1"/>
-      <c r="V51" s="1"/>
-      <c r="W51" s="1"/>
-      <c r="X51" s="1"/>
-      <c r="Y51" s="1"/>
-      <c r="Z51" s="1"/>
-      <c r="AA51" s="1"/>
-      <c r="AB51" s="1"/>
-      <c r="AC51" s="1"/>
-      <c r="AD51" s="1"/>
-      <c r="AE51" s="1"/>
-      <c r="AF51" s="1"/>
-      <c r="AG51" s="2"/>
-    </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>4</v>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
-      <c r="S52" s="1"/>
-      <c r="T52" s="1"/>
-      <c r="U52" s="1"/>
-      <c r="V52" s="1"/>
-      <c r="W52" s="1"/>
-      <c r="X52" s="1"/>
-      <c r="Y52" s="1"/>
-      <c r="Z52" s="1"/>
-      <c r="AA52" s="1"/>
-      <c r="AB52" s="1"/>
-      <c r="AC52" s="3"/>
-      <c r="AD52" s="1"/>
-      <c r="AE52" s="1"/>
-      <c r="AF52" s="1"/>
-      <c r="AG52" s="2"/>
-    </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>5</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
-      <c r="S53" s="1"/>
-      <c r="T53" s="1"/>
-      <c r="U53" s="1"/>
-      <c r="V53" s="1"/>
-      <c r="W53" s="1"/>
-      <c r="X53" s="1"/>
-      <c r="Y53" s="1"/>
-      <c r="Z53" s="1"/>
-      <c r="AA53" s="1"/>
-      <c r="AB53" s="1"/>
-      <c r="AC53" s="1"/>
-      <c r="AD53" s="1"/>
-      <c r="AE53" s="1"/>
-      <c r="AF53" s="1"/>
-      <c r="AG53" s="2"/>
-    </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>6</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-      <c r="T54" s="1"/>
-      <c r="U54" s="1"/>
-      <c r="V54" s="1"/>
-      <c r="W54" s="1"/>
-      <c r="X54" s="1"/>
-      <c r="Y54" s="1"/>
-      <c r="Z54" s="1"/>
-      <c r="AA54" s="1"/>
-      <c r="AB54" s="1"/>
-      <c r="AC54" s="1"/>
-      <c r="AD54" s="1"/>
-      <c r="AE54" s="1"/>
-      <c r="AF54" s="1"/>
-      <c r="AG54" s="2"/>
-    </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>7</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="3">
-        <v>3</v>
-      </c>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1"/>
-      <c r="U55" s="1"/>
-      <c r="V55" s="1"/>
-      <c r="W55" s="1"/>
-      <c r="X55" s="1"/>
-      <c r="Y55" s="1"/>
-      <c r="Z55" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA55" s="1"/>
-      <c r="AB55" s="1"/>
-      <c r="AC55" s="1"/>
-      <c r="AD55" s="1"/>
-      <c r="AE55" s="1"/>
-      <c r="AF55" s="1"/>
-      <c r="AG55" s="2"/>
-    </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>8</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="1"/>
-      <c r="T56" s="1"/>
-      <c r="U56" s="1"/>
-      <c r="V56" s="1"/>
-      <c r="W56" s="1"/>
-      <c r="X56" s="1"/>
-      <c r="Y56" s="1"/>
-      <c r="Z56" s="1"/>
-      <c r="AA56" s="1"/>
-      <c r="AB56" s="1"/>
-      <c r="AC56" s="1"/>
-      <c r="AD56" s="1"/>
-      <c r="AE56" s="1"/>
-      <c r="AF56" s="1"/>
-      <c r="AG56" s="2"/>
-    </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>9</v>
-      </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
-      <c r="S57" s="1"/>
-      <c r="T57" s="1"/>
-      <c r="U57" s="1"/>
-      <c r="V57" s="1"/>
-      <c r="W57" s="1"/>
-      <c r="X57" s="1"/>
-      <c r="Y57" s="1"/>
-      <c r="Z57" s="1"/>
-      <c r="AA57" s="1"/>
-      <c r="AB57" s="1"/>
-      <c r="AC57" s="1"/>
-      <c r="AD57" s="1"/>
-      <c r="AE57" s="1"/>
-      <c r="AF57" s="1"/>
-      <c r="AG57" s="2"/>
-    </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>10</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="1"/>
-      <c r="T58" s="1"/>
-      <c r="U58" s="1"/>
-      <c r="V58" s="1"/>
-      <c r="W58" s="3"/>
-      <c r="X58" s="1"/>
-      <c r="Y58" s="1"/>
-      <c r="Z58" s="1"/>
-      <c r="AA58" s="1"/>
-      <c r="AB58" s="1"/>
-      <c r="AC58" s="1"/>
-      <c r="AD58" s="1"/>
-      <c r="AE58" s="1"/>
-      <c r="AF58" s="1"/>
-      <c r="AG58" s="2"/>
-    </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>11</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
-      <c r="S59" s="1"/>
-      <c r="T59" s="1"/>
-      <c r="U59" s="1"/>
-      <c r="V59" s="1"/>
-      <c r="W59" s="1"/>
-      <c r="X59" s="1"/>
-      <c r="Y59" s="1"/>
-      <c r="Z59" s="1"/>
-      <c r="AA59" s="1"/>
-      <c r="AB59" s="1"/>
-      <c r="AC59" s="1"/>
-      <c r="AD59" s="1"/>
-      <c r="AE59" s="1"/>
-      <c r="AF59" s="1"/>
-      <c r="AG59" s="2"/>
-    </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>12</v>
-      </c>
-      <c r="B60" s="2"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
-      <c r="S60" s="1"/>
-      <c r="T60" s="1"/>
-      <c r="U60" s="1"/>
-      <c r="V60" s="1"/>
-      <c r="W60" s="1"/>
-      <c r="X60" s="1"/>
-      <c r="Y60" s="1"/>
-      <c r="Z60" s="1"/>
-      <c r="AA60" s="1"/>
-      <c r="AB60" s="1"/>
-      <c r="AC60" s="1"/>
-      <c r="AD60" s="1"/>
-      <c r="AE60" s="1"/>
-      <c r="AF60" s="1"/>
-      <c r="AG60" s="2"/>
-    </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>13</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-      <c r="S61" s="1"/>
-      <c r="T61" s="3">
-        <v>1</v>
-      </c>
-      <c r="U61" s="1"/>
-      <c r="V61" s="1"/>
-      <c r="W61" s="1"/>
-      <c r="X61" s="1"/>
-      <c r="Y61" s="1"/>
-      <c r="Z61" s="1"/>
-      <c r="AA61" s="1"/>
-      <c r="AB61" s="1"/>
-      <c r="AC61" s="1"/>
-      <c r="AD61" s="1"/>
-      <c r="AE61" s="1"/>
-      <c r="AF61" s="1"/>
-      <c r="AG61" s="2"/>
-    </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>14</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
-      <c r="S62" s="1"/>
-      <c r="T62" s="1"/>
-      <c r="U62" s="1"/>
-      <c r="V62" s="1"/>
-      <c r="W62" s="1"/>
-      <c r="X62" s="1"/>
-      <c r="Y62" s="1"/>
-      <c r="Z62" s="1"/>
-      <c r="AA62" s="1"/>
-      <c r="AB62" s="1"/>
-      <c r="AC62" s="1"/>
-      <c r="AD62" s="1"/>
-      <c r="AE62" s="1"/>
-      <c r="AF62" s="1"/>
-      <c r="AG62" s="2"/>
-    </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>15</v>
-      </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1"/>
-      <c r="V63" s="1"/>
-      <c r="W63" s="1"/>
-      <c r="X63" s="1"/>
-      <c r="Y63" s="1"/>
-      <c r="Z63" s="1"/>
-      <c r="AA63" s="1"/>
-      <c r="AB63" s="1"/>
-      <c r="AC63" s="1"/>
-      <c r="AD63" s="1"/>
-      <c r="AE63" s="1"/>
-      <c r="AF63" s="1"/>
-      <c r="AG63" s="2"/>
-    </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>16</v>
-      </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-      <c r="T64" s="1"/>
-      <c r="U64" s="1"/>
-      <c r="V64" s="1"/>
-      <c r="W64" s="1"/>
-      <c r="X64" s="1"/>
-      <c r="Y64" s="1"/>
-      <c r="Z64" s="1"/>
-      <c r="AA64" s="1"/>
-      <c r="AB64" s="1"/>
-      <c r="AC64" s="1"/>
-      <c r="AD64" s="1"/>
-      <c r="AE64" s="1"/>
-      <c r="AF64" s="1"/>
-      <c r="AG64" s="2"/>
-    </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>17</v>
-      </c>
-      <c r="B65" s="2"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-      <c r="S65" s="1"/>
-      <c r="T65" s="1"/>
-      <c r="U65" s="1"/>
-      <c r="V65" s="1"/>
-      <c r="W65" s="1"/>
-      <c r="X65" s="1"/>
-      <c r="Y65" s="1"/>
-      <c r="Z65" s="1"/>
-      <c r="AA65" s="1"/>
-      <c r="AB65" s="1"/>
-      <c r="AC65" s="1"/>
-      <c r="AD65" s="1"/>
-      <c r="AE65" s="1"/>
-      <c r="AF65" s="1"/>
-      <c r="AG65" s="2"/>
-    </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>18</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="3">
-        <v>2</v>
-      </c>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="3"/>
-      <c r="R66" s="1"/>
-      <c r="S66" s="1"/>
-      <c r="T66" s="1"/>
-      <c r="U66" s="1"/>
-      <c r="V66" s="1"/>
-      <c r="W66" s="1"/>
-      <c r="X66" s="1"/>
-      <c r="Y66" s="1"/>
-      <c r="Z66" s="1"/>
-      <c r="AA66" s="1"/>
-      <c r="AB66" s="1"/>
-      <c r="AC66" s="1"/>
-      <c r="AD66" s="1"/>
-      <c r="AE66" s="1"/>
-      <c r="AF66" s="1"/>
-      <c r="AG66" s="2"/>
-    </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>19</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1"/>
-      <c r="W67" s="1"/>
-      <c r="X67" s="1"/>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="1"/>
-      <c r="AB67" s="1"/>
-      <c r="AC67" s="1"/>
-      <c r="AD67" s="1"/>
-      <c r="AE67" s="1"/>
-      <c r="AF67" s="1"/>
-      <c r="AG67" s="2"/>
-    </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>20</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
-      <c r="U68" s="1"/>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="X68" s="1"/>
-      <c r="Y68" s="1"/>
-      <c r="Z68" s="1"/>
-      <c r="AA68" s="1"/>
-      <c r="AB68" s="1"/>
-      <c r="AC68" s="1"/>
-      <c r="AD68" s="1"/>
-      <c r="AE68" s="1"/>
-      <c r="AF68" s="1"/>
-      <c r="AG68" s="2"/>
-    </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>21</v>
-      </c>
-      <c r="B69" s="2"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="3">
-        <v>1</v>
-      </c>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="3">
-        <v>1</v>
-      </c>
-      <c r="U69" s="1"/>
-      <c r="V69" s="1"/>
-      <c r="W69" s="1"/>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="1"/>
-      <c r="AA69" s="1"/>
-      <c r="AB69" s="1"/>
-      <c r="AC69" s="1"/>
-      <c r="AD69" s="1"/>
-      <c r="AE69" s="1"/>
-      <c r="AF69" s="1"/>
-      <c r="AG69" s="2"/>
-    </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>22</v>
-      </c>
-      <c r="B70" s="2"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-      <c r="T70" s="1"/>
-      <c r="U70" s="1"/>
-      <c r="V70" s="1"/>
-      <c r="W70" s="1"/>
-      <c r="X70" s="1"/>
-      <c r="Y70" s="1"/>
-      <c r="Z70" s="1"/>
-      <c r="AA70" s="1"/>
-      <c r="AB70" s="1"/>
-      <c r="AC70" s="1"/>
-      <c r="AD70" s="1"/>
-      <c r="AE70" s="1"/>
-      <c r="AF70" s="1"/>
-      <c r="AG70" s="2"/>
-    </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>23</v>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
-      <c r="N71" s="1"/>
-      <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
-      <c r="T71" s="1"/>
-      <c r="U71" s="1"/>
-      <c r="V71" s="1"/>
-      <c r="W71" s="1"/>
-      <c r="X71" s="1"/>
-      <c r="Y71" s="1"/>
-      <c r="Z71" s="1"/>
-      <c r="AA71" s="1"/>
-      <c r="AB71" s="1"/>
-      <c r="AC71" s="1"/>
-      <c r="AD71" s="1"/>
-      <c r="AE71" s="1"/>
-      <c r="AF71" s="1"/>
-      <c r="AG71" s="2"/>
-    </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>24</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="1"/>
-      <c r="R72" s="1"/>
-      <c r="S72" s="1"/>
-      <c r="T72" s="1"/>
-      <c r="U72" s="1"/>
-      <c r="V72" s="1"/>
-      <c r="W72" s="3">
-        <v>3</v>
-      </c>
-      <c r="X72" s="1"/>
-      <c r="Y72" s="1"/>
-      <c r="Z72" s="1"/>
-      <c r="AA72" s="1"/>
-      <c r="AB72" s="1"/>
-      <c r="AC72" s="1"/>
-      <c r="AD72" s="1"/>
-      <c r="AE72" s="1"/>
-      <c r="AF72" s="1"/>
-      <c r="AG72" s="2"/>
-    </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>25</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
-      <c r="R73" s="1"/>
-      <c r="S73" s="1"/>
-      <c r="T73" s="1"/>
-      <c r="U73" s="1"/>
-      <c r="V73" s="1"/>
-      <c r="W73" s="1"/>
-      <c r="X73" s="1"/>
-      <c r="Y73" s="1"/>
-      <c r="Z73" s="1"/>
-      <c r="AA73" s="1"/>
-      <c r="AB73" s="1"/>
-      <c r="AC73" s="1"/>
-      <c r="AD73" s="1"/>
-      <c r="AE73" s="1"/>
-      <c r="AF73" s="1"/>
-      <c r="AG73" s="2"/>
-    </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>26</v>
-      </c>
-      <c r="B74" s="2"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="1"/>
-      <c r="T74" s="1"/>
-      <c r="U74" s="1"/>
-      <c r="V74" s="1"/>
-      <c r="W74" s="1"/>
-      <c r="X74" s="1"/>
-      <c r="Y74" s="1"/>
-      <c r="Z74" s="1"/>
-      <c r="AA74" s="1"/>
-      <c r="AB74" s="1"/>
-      <c r="AC74" s="1"/>
-      <c r="AD74" s="1"/>
-      <c r="AE74" s="1"/>
-      <c r="AF74" s="1"/>
-      <c r="AG74" s="2"/>
-    </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>27</v>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="3">
-        <v>2</v>
-      </c>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-      <c r="S75" s="1"/>
-      <c r="T75" s="1"/>
-      <c r="U75" s="1"/>
-      <c r="V75" s="1"/>
-      <c r="W75" s="1"/>
-      <c r="X75" s="1"/>
-      <c r="Y75" s="1"/>
-      <c r="Z75" s="3"/>
-      <c r="AA75" s="1"/>
-      <c r="AB75" s="1"/>
-      <c r="AC75" s="1"/>
-      <c r="AD75" s="1"/>
-      <c r="AE75" s="1"/>
-      <c r="AF75" s="1"/>
-      <c r="AG75" s="2"/>
-    </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>28</v>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-      <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
-      <c r="S76" s="1"/>
-      <c r="T76" s="1"/>
-      <c r="U76" s="1"/>
-      <c r="V76" s="1"/>
-      <c r="W76" s="1"/>
-      <c r="X76" s="1"/>
-      <c r="Y76" s="1"/>
-      <c r="Z76" s="1"/>
-      <c r="AA76" s="1"/>
-      <c r="AB76" s="1"/>
-      <c r="AC76" s="1"/>
-      <c r="AD76" s="1"/>
-      <c r="AE76" s="1"/>
-      <c r="AF76" s="1"/>
-      <c r="AG76" s="2"/>
-    </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>29</v>
-      </c>
-      <c r="B77" s="2"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
-      <c r="S77" s="1"/>
-      <c r="T77" s="1"/>
-      <c r="U77" s="1"/>
-      <c r="V77" s="1"/>
-      <c r="W77" s="1"/>
-      <c r="X77" s="1"/>
-      <c r="Y77" s="1"/>
-      <c r="Z77" s="1"/>
-      <c r="AA77" s="1"/>
-      <c r="AB77" s="1"/>
-      <c r="AC77" s="1"/>
-      <c r="AD77" s="1"/>
-      <c r="AE77" s="1"/>
-      <c r="AF77" s="1"/>
-      <c r="AG77" s="2"/>
-    </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>30</v>
-      </c>
-      <c r="B78" s="2"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
-      <c r="M78" s="1"/>
-      <c r="N78" s="1"/>
-      <c r="O78" s="1"/>
-      <c r="P78" s="1"/>
-      <c r="Q78" s="1"/>
-      <c r="R78" s="1"/>
-      <c r="S78" s="1"/>
-      <c r="T78" s="1"/>
-      <c r="U78" s="1"/>
-      <c r="V78" s="1"/>
-      <c r="W78" s="1"/>
-      <c r="X78" s="1"/>
-      <c r="Y78" s="1"/>
-      <c r="Z78" s="1"/>
-      <c r="AA78" s="1"/>
-      <c r="AB78" s="1"/>
-      <c r="AC78" s="5"/>
-      <c r="AD78" s="1"/>
-      <c r="AE78" s="1"/>
-      <c r="AF78" s="1"/>
-      <c r="AG78" s="2"/>
-    </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B79" s="1"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2"/>
-      <c r="N79" s="2"/>
-      <c r="O79" s="2"/>
-      <c r="P79" s="2"/>
-      <c r="Q79" s="2"/>
-      <c r="R79" s="2"/>
-      <c r="S79" s="2"/>
-      <c r="T79" s="2"/>
-      <c r="U79" s="2"/>
-      <c r="V79" s="2"/>
-      <c r="W79" s="2"/>
-      <c r="X79" s="2"/>
-      <c r="Y79" s="2"/>
-      <c r="Z79" s="2"/>
-      <c r="AA79" s="2"/>
-      <c r="AB79" s="2"/>
-      <c r="AC79" s="2"/>
-      <c r="AD79" s="2"/>
-      <c r="AE79" s="2"/>
-      <c r="AF79" s="2"/>
-      <c r="AG79" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>